<commit_message>
add . to each line
</commit_message>
<xml_diff>
--- a/升级测试模板.xlsx
+++ b/升级测试模板.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -42,31 +42,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.在服务器上上传最新版本的测试包或者提高版本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2.安装低版本进行升级测试</t>
+    <t>VX.X（旧版本）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.在服务器上上传最新版本的测试包或者提高版本。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.安装低版本进行升级测试。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>3.主要测试方向：
-A.查看是否弹出升级提示
-B.如果启动画面有修改升级后需要对最新画面全部展示
-C.升级后必须依然是已经登录状态
-D.升级后新增/修改的功能是否能够正确实现</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VX.X（旧版本）</t>
+A.查看是否弹出升级提示。
+B.如果启动画面有修改升级后需要对最新画面全部展示。
+C.升级后必须依然是已经登录状态。
+D.升级后新增/修改的功能是否能够正确实现。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,11 +161,16 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -239,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -273,6 +279,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -448,14 +455,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="57.375" customWidth="1"/>
@@ -463,24 +470,24 @@
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:2" ht="16.5">
+    <row r="3" spans="2:2" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="67.5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -491,20 +498,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -518,9 +525,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -528,61 +535,61 @@
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -596,12 +603,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>